<commit_message>
Keep the necessary files
</commit_message>
<xml_diff>
--- a/round1984.xlsx
+++ b/round1984.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa5fe2a5bf147a6/Desktop/Green LLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_AD4DA82427541F7ACA7EB8BAF849363E6BE8DE10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9E2BDE9-ACA0-4C10-B53E-984E0B617E75}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_AD4DA82427541F7ACA7EB8BAF849363E6BE8DE10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FB8F792-12DA-4658-A480-3C53AABE5B6E}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -522,12 +522,12 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -919,7 +919,7 @@
       </c>
       <c r="G17">
         <f>SUM(B17:F17)</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -972,7 +972,7 @@
       </c>
       <c r="G19">
         <f>SUM(B19:F19)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
@@ -1014,11 +1014,11 @@
       </c>
       <c r="B21">
         <f>(B17+B19)*$L$20</f>
-        <v>5.4999999999999993E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="C21" s="8">
         <f>(C17+C19)*$L$20</f>
-        <v>6.6000000000000003E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D21">
         <f>(D17+D19)*$L$20</f>
@@ -1136,11 +1136,11 @@
       </c>
       <c r="B25">
         <f>B21+(B22+B24)*$L$2*$N$2</f>
-        <v>5.4999999999999993E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="C25" s="4">
         <f>C21+(C22+C24)*$L$2*$N$2</f>
-        <v>6.6618110077821008E-2</v>
+        <v>7.7618110077821004E-2</v>
       </c>
       <c r="D25" s="4">
         <f>D21+(D22+D24)*$L$2*$N$2</f>
@@ -1168,11 +1168,11 @@
       </c>
       <c r="B26">
         <f>B25*$L$25</f>
-        <v>11.934999999999999</v>
+        <v>9.548</v>
       </c>
       <c r="C26" s="8">
         <f t="shared" ref="C26:F26" si="6">C25*$L$25</f>
-        <v>14.456129886887158</v>
+        <v>16.843129886887159</v>
       </c>
       <c r="D26" s="8">
         <f t="shared" si="6"/>

</xml_diff>